<commit_message>
Fee details page have been updated
</commit_message>
<xml_diff>
--- a/Import Fee Details/HarishFebruary.xlsx
+++ b/Import Fee Details/HarishFebruary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Guardian Portal System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Guardian Portal System\Import Fee Details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029B0EBB-4842-4B79-8439-0AE2EFF3EC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CBFF4B-8CE7-451B-9031-4E93866C8AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2411D16-9995-4C86-B65F-C09FE3B757C5}"/>
   </bookViews>
@@ -425,6 +425,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>